<commit_message>
Commit atualizando tesouro dia 22/05
</commit_message>
<xml_diff>
--- a/TESOURO DIRETO_0419 - Compra.xlsx
+++ b/TESOURO DIRETO_0419 - Compra.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RHF Talentos\Downloads\tesouroDireto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Suporte\Downloads\tesouro\tesourodireto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -160,10 +160,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
-    <numFmt numFmtId="164" formatCode="&quot;R$&quot;#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="dd/mm"/>
-    <numFmt numFmtId="166" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00"/>
+    <numFmt numFmtId="8" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="&quot;R$&quot;#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="dd/mm"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -859,7 +859,7 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -878,43 +878,43 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="6" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="6" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="6" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -938,7 +938,7 @@
     <xf numFmtId="14" fontId="6" fillId="7" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="8" fontId="9" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -953,31 +953,31 @@
     <xf numFmtId="14" fontId="6" fillId="7" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="7" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="7" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="9" fillId="10" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="10" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="9" fillId="10" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="10" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="9" fillId="10" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="10" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="7" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="7" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -998,7 +998,7 @@
     <xf numFmtId="0" fontId="9" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="9" fillId="10" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="10" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1028,7 +1028,7 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="7" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="6" fillId="7" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="9" fillId="10" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1073,10 +1073,10 @@
     <xf numFmtId="14" fontId="6" fillId="7" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="7" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="7" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="7" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="7" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="9" fillId="10" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2864,11 +2864,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="355871320"/>
-        <c:axId val="3384352"/>
+        <c:axId val="289801744"/>
+        <c:axId val="289805552"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="355871320"/>
+        <c:axId val="289801744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2910,7 +2910,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3384352"/>
+        <c:crossAx val="289805552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2918,7 +2918,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="3384352"/>
+        <c:axId val="289805552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2968,7 +2968,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="355871320"/>
+        <c:crossAx val="289801744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3381,8 +3381,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="357777512"/>
-        <c:axId val="357777904"/>
+        <c:axId val="175746480"/>
+        <c:axId val="175745392"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -3919,7 +3919,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="357777512"/>
+        <c:axId val="175746480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3953,7 +3953,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="357777904"/>
+        <c:crossAx val="175745392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3961,7 +3961,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="357777904"/>
+        <c:axId val="175745392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3971,7 +3971,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="357777512"/>
+        <c:crossAx val="175746480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4305,34 +4305,34 @@
                 <c:pt idx="2">
                   <c:v>30.14</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>30.09</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>30.03</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>39.950000000000003</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>30.2</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>30.45</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>30.54</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>30.4</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>31.02</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>30.65</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>30.98</c:v>
                 </c:pt>
               </c:numCache>
@@ -4371,8 +4371,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="357778688"/>
-        <c:axId val="357779080"/>
+        <c:axId val="175736688"/>
+        <c:axId val="175738320"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -4604,34 +4604,34 @@
                       <c:pt idx="2">
                         <c:v>51.45</c:v>
                       </c:pt>
-                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>51.44</c:v>
                       </c:pt>
-                      <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>51.51</c:v>
                       </c:pt>
-                      <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>51.55</c:v>
                       </c:pt>
-                      <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>51.57</c:v>
                       </c:pt>
-                      <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>51.69</c:v>
                       </c:pt>
-                      <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>51.77</c:v>
                       </c:pt>
-                      <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>51.78</c:v>
                       </c:pt>
-                      <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>51.96</c:v>
                       </c:pt>
-                      <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>51.77</c:v>
                       </c:pt>
-                      <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>51.84</c:v>
                       </c:pt>
                     </c:numCache>
@@ -4869,34 +4869,34 @@
                       <c:pt idx="2">
                         <c:v>31.34</c:v>
                       </c:pt>
-                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>31.32</c:v>
                       </c:pt>
-                      <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>31.29</c:v>
                       </c:pt>
-                      <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>31.25</c:v>
                       </c:pt>
-                      <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>31.41</c:v>
                       </c:pt>
-                      <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>31.58</c:v>
                       </c:pt>
-                      <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>31.64</c:v>
                       </c:pt>
-                      <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>31.55</c:v>
                       </c:pt>
-                      <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>31.95</c:v>
                       </c:pt>
-                      <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>31.72</c:v>
                       </c:pt>
-                      <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>31.95</c:v>
                       </c:pt>
                     </c:numCache>
@@ -4909,7 +4909,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="357778688"/>
+        <c:axId val="175736688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4943,7 +4943,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="357779080"/>
+        <c:crossAx val="175738320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4951,7 +4951,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="357779080"/>
+        <c:axId val="175738320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4961,7 +4961,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="357778688"/>
+        <c:crossAx val="175736688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5900,11 +5900,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="357779864"/>
-        <c:axId val="357780256"/>
+        <c:axId val="175737776"/>
+        <c:axId val="175739408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="357779864"/>
+        <c:axId val="175737776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5947,7 +5947,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="357780256"/>
+        <c:crossAx val="175739408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5955,7 +5955,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="357780256"/>
+        <c:axId val="175739408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5965,7 +5965,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="357779864"/>
+        <c:crossAx val="175737776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6060,7 +6060,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6165,7 +6164,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -6302,34 +6300,34 @@
                 <c:pt idx="2">
                   <c:v>3584.21</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>3581.12</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>3582.35</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>3581.51</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>3580.66</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>3585.91</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>3593.4</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>3594.64</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>3608.42</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>3597.11</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>3604.98</c:v>
                 </c:pt>
               </c:numCache>
@@ -6368,11 +6366,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="358025808"/>
-        <c:axId val="358026200"/>
+        <c:axId val="175749200"/>
+        <c:axId val="175742128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="358025808"/>
+        <c:axId val="175749200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6406,7 +6404,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358026200"/>
+        <c:crossAx val="175742128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6414,7 +6412,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="358026200"/>
+        <c:axId val="175742128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6424,7 +6422,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="358025808"/>
+        <c:crossAx val="175749200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6438,7 +6436,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6516,7 +6513,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6621,7 +6617,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -6758,34 +6753,34 @@
                 <c:pt idx="2">
                   <c:v>3833.59</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>3833.06</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>3830.46</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>3827.87</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>3837.13</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>3852.46</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>3857.8</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>3855.18</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>3888.54</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>3865.86</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>3885.88</c:v>
                 </c:pt>
               </c:numCache>
@@ -6824,8 +6819,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="358026984"/>
-        <c:axId val="358027376"/>
+        <c:axId val="175735056"/>
+        <c:axId val="175740496"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -7057,34 +7052,34 @@
                       <c:pt idx="2">
                         <c:v>3584.21</c:v>
                       </c:pt>
-                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>3581.12</c:v>
                       </c:pt>
-                      <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>3582.35</c:v>
                       </c:pt>
-                      <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>3581.51</c:v>
                       </c:pt>
-                      <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>3580.66</c:v>
                       </c:pt>
-                      <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>3585.91</c:v>
                       </c:pt>
-                      <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>3593.4</c:v>
                       </c:pt>
-                      <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>3594.64</c:v>
                       </c:pt>
-                      <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>3608.42</c:v>
                       </c:pt>
-                      <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>3597.11</c:v>
                       </c:pt>
-                      <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>3604.98</c:v>
                       </c:pt>
                     </c:numCache>
@@ -7322,34 +7317,34 @@
                       <c:pt idx="2">
                         <c:v>3980.83</c:v>
                       </c:pt>
-                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>3990.52</c:v>
                       </c:pt>
-                      <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>3991.94</c:v>
                       </c:pt>
-                      <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>3981.17</c:v>
                       </c:pt>
-                      <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>3988.68</c:v>
                       </c:pt>
-                      <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>4010.64</c:v>
                       </c:pt>
-                      <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>4018.22</c:v>
                       </c:pt>
-                      <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>4019.65</c:v>
                       </c:pt>
-                      <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>4058.32</c:v>
                       </c:pt>
-                      <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>4022.51</c:v>
                       </c:pt>
-                      <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>4051.49</c:v>
                       </c:pt>
                     </c:numCache>
@@ -7362,7 +7357,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="358026984"/>
+        <c:axId val="175735056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7396,7 +7391,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358027376"/>
+        <c:crossAx val="175740496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7404,7 +7399,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="358027376"/>
+        <c:axId val="175740496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7414,7 +7409,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="358026984"/>
+        <c:crossAx val="175735056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7428,7 +7423,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7506,7 +7500,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7611,7 +7604,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -7748,34 +7740,34 @@
                 <c:pt idx="2">
                   <c:v>3980.83</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>3990.52</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>3991.94</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>3981.17</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>3988.68</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>4010.64</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>4018.22</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>4019.65</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>4058.32</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>4022.51</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>4051.49</c:v>
                 </c:pt>
               </c:numCache>
@@ -7814,8 +7806,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="358028160"/>
-        <c:axId val="358028552"/>
+        <c:axId val="289796304"/>
+        <c:axId val="289798480"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -8047,34 +8039,34 @@
                       <c:pt idx="2">
                         <c:v>3584.21</c:v>
                       </c:pt>
-                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>3581.12</c:v>
                       </c:pt>
-                      <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>3582.35</c:v>
                       </c:pt>
-                      <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>3581.51</c:v>
                       </c:pt>
-                      <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>3580.66</c:v>
                       </c:pt>
-                      <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>3585.91</c:v>
                       </c:pt>
-                      <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>3593.4</c:v>
                       </c:pt>
-                      <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>3594.64</c:v>
                       </c:pt>
-                      <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>3608.42</c:v>
                       </c:pt>
-                      <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>3597.11</c:v>
                       </c:pt>
-                      <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>3604.98</c:v>
                       </c:pt>
                     </c:numCache>
@@ -8312,34 +8304,34 @@
                       <c:pt idx="2">
                         <c:v>3833.59</c:v>
                       </c:pt>
-                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>3833.06</c:v>
                       </c:pt>
-                      <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>3830.46</c:v>
                       </c:pt>
-                      <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>3827.87</c:v>
                       </c:pt>
-                      <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>3837.13</c:v>
                       </c:pt>
-                      <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>3852.46</c:v>
                       </c:pt>
-                      <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>3857.8</c:v>
                       </c:pt>
-                      <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>3855.18</c:v>
                       </c:pt>
-                      <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>3888.54</c:v>
                       </c:pt>
-                      <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>3865.86</c:v>
                       </c:pt>
-                      <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>3885.88</c:v>
                       </c:pt>
                     </c:numCache>
@@ -8352,7 +8344,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="358028160"/>
+        <c:axId val="289796304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8386,7 +8378,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358028552"/>
+        <c:crossAx val="289798480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8394,7 +8386,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="358028552"/>
+        <c:axId val="289798480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8404,7 +8396,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="358028160"/>
+        <c:crossAx val="289796304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8418,7 +8410,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8496,7 +8487,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8601,7 +8591,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -8738,34 +8727,34 @@
                 <c:pt idx="2">
                   <c:v>39.799999999999997</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>39.9</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>39.909999999999997</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>39.81</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>39.880000000000003</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>40.1</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>40.18</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>40.19</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>40.58</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>40.22</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>40.51</c:v>
                 </c:pt>
               </c:numCache>
@@ -8804,8 +8793,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="358749864"/>
-        <c:axId val="358750256"/>
+        <c:axId val="289797392"/>
+        <c:axId val="289797936"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -9037,34 +9026,34 @@
                       <c:pt idx="2">
                         <c:v>35.840000000000003</c:v>
                       </c:pt>
-                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>35.81</c:v>
                       </c:pt>
-                      <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>35.82</c:v>
                       </c:pt>
-                      <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>35.81</c:v>
                       </c:pt>
-                      <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>35.799999999999997</c:v>
                       </c:pt>
-                      <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>35.85</c:v>
                       </c:pt>
-                      <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>35.93</c:v>
                       </c:pt>
-                      <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>35.94</c:v>
                       </c:pt>
-                      <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>36.08</c:v>
                       </c:pt>
-                      <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>35.97</c:v>
                       </c:pt>
-                      <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>36.04</c:v>
                       </c:pt>
                     </c:numCache>
@@ -9302,34 +9291,34 @@
                       <c:pt idx="2">
                         <c:v>38.33</c:v>
                       </c:pt>
-                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>38.33</c:v>
                       </c:pt>
-                      <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>38.299999999999997</c:v>
                       </c:pt>
-                      <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>38.270000000000003</c:v>
                       </c:pt>
-                      <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>38.369999999999997</c:v>
                       </c:pt>
-                      <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>38.520000000000003</c:v>
                       </c:pt>
-                      <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>38.57</c:v>
                       </c:pt>
-                      <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>38.549999999999997</c:v>
                       </c:pt>
-                      <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>38.880000000000003</c:v>
                       </c:pt>
-                      <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>38.65</c:v>
                       </c:pt>
-                      <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>38.85</c:v>
                       </c:pt>
                     </c:numCache>
@@ -9342,7 +9331,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="358749864"/>
+        <c:axId val="289797392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9376,7 +9365,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358750256"/>
+        <c:crossAx val="289797936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9384,7 +9373,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="358750256"/>
+        <c:axId val="289797936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9394,7 +9383,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="358749864"/>
+        <c:crossAx val="289797392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9408,7 +9397,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9486,7 +9474,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9591,7 +9578,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -9728,34 +9714,34 @@
                 <c:pt idx="2">
                   <c:v>38.33</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>38.33</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>38.299999999999997</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>38.270000000000003</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>38.369999999999997</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>38.520000000000003</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>38.57</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>38.549999999999997</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>38.880000000000003</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>38.65</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>38.85</c:v>
                 </c:pt>
               </c:numCache>
@@ -9794,8 +9780,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="358751040"/>
-        <c:axId val="358751432"/>
+        <c:axId val="174025088"/>
+        <c:axId val="174015840"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -10027,34 +10013,34 @@
                       <c:pt idx="2">
                         <c:v>35.840000000000003</c:v>
                       </c:pt>
-                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>35.81</c:v>
                       </c:pt>
-                      <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>35.82</c:v>
                       </c:pt>
-                      <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>35.81</c:v>
                       </c:pt>
-                      <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>35.799999999999997</c:v>
                       </c:pt>
-                      <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>35.85</c:v>
                       </c:pt>
-                      <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>35.93</c:v>
                       </c:pt>
-                      <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>35.94</c:v>
                       </c:pt>
-                      <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>36.08</c:v>
                       </c:pt>
-                      <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>35.97</c:v>
                       </c:pt>
-                      <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>36.04</c:v>
                       </c:pt>
                     </c:numCache>
@@ -10292,34 +10278,34 @@
                       <c:pt idx="2">
                         <c:v>39.799999999999997</c:v>
                       </c:pt>
-                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>39.9</c:v>
                       </c:pt>
-                      <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>39.909999999999997</c:v>
                       </c:pt>
-                      <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>39.81</c:v>
                       </c:pt>
-                      <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>39.880000000000003</c:v>
                       </c:pt>
-                      <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>40.1</c:v>
                       </c:pt>
-                      <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>40.18</c:v>
                       </c:pt>
-                      <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>40.19</c:v>
                       </c:pt>
-                      <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>40.58</c:v>
                       </c:pt>
-                      <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>40.22</c:v>
                       </c:pt>
-                      <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>40.51</c:v>
                       </c:pt>
                     </c:numCache>
@@ -10332,7 +10318,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="358751040"/>
+        <c:axId val="174025088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10366,7 +10352,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358751432"/>
+        <c:crossAx val="174015840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10374,7 +10360,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="358751432"/>
+        <c:axId val="174015840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10384,7 +10370,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="358751040"/>
+        <c:crossAx val="174025088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10398,7 +10384,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10476,7 +10461,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10581,7 +10565,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -10718,34 +10701,34 @@
                 <c:pt idx="2">
                   <c:v>35.840000000000003</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>35.81</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>35.82</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>35.81</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>35.799999999999997</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>35.85</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>35.93</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>35.94</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>36.08</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>35.97</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>36.04</c:v>
                 </c:pt>
               </c:numCache>
@@ -10784,11 +10767,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="358752216"/>
-        <c:axId val="358752608"/>
+        <c:axId val="2094128848"/>
+        <c:axId val="2094126672"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="358752216"/>
+        <c:axId val="2094128848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10822,7 +10805,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358752608"/>
+        <c:crossAx val="2094126672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10830,7 +10813,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="358752608"/>
+        <c:axId val="2094126672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10840,7 +10823,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="358752216"/>
+        <c:crossAx val="2094128848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10854,7 +10837,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10932,7 +10914,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11037,7 +11018,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -11240,8 +11220,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="358753392"/>
-        <c:axId val="358620872"/>
+        <c:axId val="177015872"/>
+        <c:axId val="196469744"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -11778,7 +11758,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="358753392"/>
+        <c:axId val="177015872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11812,7 +11792,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358620872"/>
+        <c:crossAx val="196469744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11820,7 +11800,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="358620872"/>
+        <c:axId val="196469744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11830,7 +11810,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="358753392"/>
+        <c:crossAx val="177015872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11844,7 +11824,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12555,11 +12534,11 @@
         </c:dLbls>
         <c:gapWidth val="315"/>
         <c:overlap val="-40"/>
-        <c:axId val="3347456"/>
-        <c:axId val="302899528"/>
+        <c:axId val="289803376"/>
+        <c:axId val="289793584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="3347456"/>
+        <c:axId val="289803376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12620,7 +12599,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302899528"/>
+        <c:crossAx val="289793584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12628,7 +12607,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="302899528"/>
+        <c:axId val="289793584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12689,7 +12668,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3347456"/>
+        <c:crossAx val="289803376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12786,7 +12765,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12891,7 +12869,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -13094,8 +13071,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="358621656"/>
-        <c:axId val="358622048"/>
+        <c:axId val="196470288"/>
+        <c:axId val="196468112"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -13632,7 +13609,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="358621656"/>
+        <c:axId val="196470288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13666,7 +13643,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358622048"/>
+        <c:crossAx val="196468112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13674,7 +13651,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="358622048"/>
+        <c:axId val="196468112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13684,7 +13661,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="358621656"/>
+        <c:crossAx val="196470288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13698,7 +13675,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13776,7 +13752,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13881,7 +13856,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -14084,8 +14058,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="358622832"/>
-        <c:axId val="358623224"/>
+        <c:axId val="196464304"/>
+        <c:axId val="196470832"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -14622,7 +14596,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="358622832"/>
+        <c:axId val="196464304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14656,7 +14630,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358623224"/>
+        <c:crossAx val="196470832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14664,7 +14638,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="358623224"/>
+        <c:axId val="196470832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14674,7 +14648,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="358622832"/>
+        <c:crossAx val="196464304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14688,7 +14662,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15072,8 +15045,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="358623616"/>
-        <c:axId val="358624400"/>
+        <c:axId val="196474096"/>
+        <c:axId val="196479536"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -15610,7 +15583,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="358623616"/>
+        <c:axId val="196474096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15644,7 +15617,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358624400"/>
+        <c:crossAx val="196479536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15652,7 +15625,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="358624400"/>
+        <c:axId val="196479536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15662,7 +15635,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="358623616"/>
+        <c:crossAx val="196474096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16059,8 +16032,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="359059536"/>
-        <c:axId val="359059928"/>
+        <c:axId val="196473008"/>
+        <c:axId val="196465392"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -16597,7 +16570,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="359059536"/>
+        <c:axId val="196473008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16631,7 +16604,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359059928"/>
+        <c:crossAx val="196465392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16639,7 +16612,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="359059928"/>
+        <c:axId val="196465392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16649,7 +16622,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="359059536"/>
+        <c:crossAx val="196473008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17046,8 +17019,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="359060712"/>
-        <c:axId val="359061104"/>
+        <c:axId val="196473552"/>
+        <c:axId val="196466480"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -17584,7 +17557,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="359060712"/>
+        <c:axId val="196473552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17618,7 +17591,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359061104"/>
+        <c:crossAx val="196466480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17626,7 +17599,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="359061104"/>
+        <c:axId val="196466480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17636,7 +17609,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="359060712"/>
+        <c:crossAx val="196473552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17967,34 +17940,34 @@
                 <c:pt idx="2">
                   <c:v>32.67</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>32.61</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>32.61</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>32.67</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>32.68</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>32.68</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>32.76</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>32.770000000000003</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>32.840000000000003</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>32.71</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>32.729999999999997</c:v>
                 </c:pt>
               </c:numCache>
@@ -18033,8 +18006,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="359061888"/>
-        <c:axId val="359062280"/>
+        <c:axId val="196475728"/>
+        <c:axId val="196476272"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -18266,34 +18239,34 @@
                       <c:pt idx="2">
                         <c:v>31.01</c:v>
                       </c:pt>
-                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>30.93</c:v>
                       </c:pt>
-                      <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>30.89</c:v>
                       </c:pt>
-                      <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>31.01</c:v>
                       </c:pt>
-                      <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>30.99</c:v>
                       </c:pt>
-                      <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>30.98</c:v>
                       </c:pt>
-                      <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>31.06</c:v>
                       </c:pt>
-                      <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>31.07</c:v>
                       </c:pt>
-                      <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>31.28</c:v>
                       </c:pt>
-                      <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>30.98</c:v>
                       </c:pt>
-                      <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>31</c:v>
                       </c:pt>
                     </c:numCache>
@@ -18531,34 +18504,34 @@
                       <c:pt idx="2">
                         <c:v>32.880000000000003</c:v>
                       </c:pt>
-                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>32.869999999999997</c:v>
                       </c:pt>
-                      <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>32.81</c:v>
                       </c:pt>
-                      <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>32.93</c:v>
                       </c:pt>
-                      <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>32.92</c:v>
                       </c:pt>
-                      <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>32.880000000000003</c:v>
                       </c:pt>
-                      <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>32.93</c:v>
                       </c:pt>
-                      <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>32.94</c:v>
                       </c:pt>
-                      <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>33.22</c:v>
                       </c:pt>
-                      <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>32.9</c:v>
                       </c:pt>
-                      <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>32.880000000000003</c:v>
                       </c:pt>
                     </c:numCache>
@@ -18571,7 +18544,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="359061888"/>
+        <c:axId val="196475728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18605,7 +18578,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359062280"/>
+        <c:crossAx val="196476272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18613,7 +18586,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="359062280"/>
+        <c:axId val="196476272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18623,7 +18596,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="359061888"/>
+        <c:crossAx val="196475728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18954,34 +18927,34 @@
                 <c:pt idx="2">
                   <c:v>31.01</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>30.93</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>30.89</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>31.01</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>30.99</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>30.98</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>31.06</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>31.07</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>31.28</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>30.98</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
@@ -19020,8 +18993,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="359310568"/>
-        <c:axId val="359310960"/>
+        <c:axId val="196468656"/>
+        <c:axId val="196465936"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -19253,34 +19226,34 @@
                       <c:pt idx="2">
                         <c:v>32.67</c:v>
                       </c:pt>
-                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>32.61</c:v>
                       </c:pt>
-                      <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>32.61</c:v>
                       </c:pt>
-                      <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>32.67</c:v>
                       </c:pt>
-                      <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>32.68</c:v>
                       </c:pt>
-                      <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>32.68</c:v>
                       </c:pt>
-                      <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>32.76</c:v>
                       </c:pt>
-                      <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>32.770000000000003</c:v>
                       </c:pt>
-                      <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>32.840000000000003</c:v>
                       </c:pt>
-                      <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>32.71</c:v>
                       </c:pt>
-                      <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>32.729999999999997</c:v>
                       </c:pt>
                     </c:numCache>
@@ -19518,34 +19491,34 @@
                       <c:pt idx="2">
                         <c:v>32.880000000000003</c:v>
                       </c:pt>
-                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>32.869999999999997</c:v>
                       </c:pt>
-                      <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>32.81</c:v>
                       </c:pt>
-                      <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>32.93</c:v>
                       </c:pt>
-                      <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>32.92</c:v>
                       </c:pt>
-                      <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>32.880000000000003</c:v>
                       </c:pt>
-                      <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>32.93</c:v>
                       </c:pt>
-                      <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>32.94</c:v>
                       </c:pt>
-                      <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>33.22</c:v>
                       </c:pt>
-                      <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>32.9</c:v>
                       </c:pt>
-                      <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>32.880000000000003</c:v>
                       </c:pt>
                     </c:numCache>
@@ -19558,7 +19531,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="359310568"/>
+        <c:axId val="196468656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19592,7 +19565,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359310960"/>
+        <c:crossAx val="196465936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -19600,7 +19573,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="359310960"/>
+        <c:axId val="196465936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19610,7 +19583,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="359310568"/>
+        <c:crossAx val="196468656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -19941,34 +19914,34 @@
                 <c:pt idx="2">
                   <c:v>32.880000000000003</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>32.869999999999997</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>32.81</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>32.93</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>32.92</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>32.880000000000003</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>32.93</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>32.94</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>33.22</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>32.9</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>32.880000000000003</c:v>
                 </c:pt>
               </c:numCache>
@@ -20007,8 +19980,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="359311744"/>
-        <c:axId val="359312136"/>
+        <c:axId val="196478448"/>
+        <c:axId val="196472464"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -20240,34 +20213,34 @@
                       <c:pt idx="2">
                         <c:v>32.67</c:v>
                       </c:pt>
-                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>32.61</c:v>
                       </c:pt>
-                      <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>32.61</c:v>
                       </c:pt>
-                      <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>32.67</c:v>
                       </c:pt>
-                      <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>32.68</c:v>
                       </c:pt>
-                      <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>32.68</c:v>
                       </c:pt>
-                      <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>32.76</c:v>
                       </c:pt>
-                      <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>32.770000000000003</c:v>
                       </c:pt>
-                      <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>32.840000000000003</c:v>
                       </c:pt>
-                      <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>32.71</c:v>
                       </c:pt>
-                      <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>32.729999999999997</c:v>
                       </c:pt>
                     </c:numCache>
@@ -20505,34 +20478,34 @@
                       <c:pt idx="2">
                         <c:v>31.01</c:v>
                       </c:pt>
-                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>30.93</c:v>
                       </c:pt>
-                      <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>30.89</c:v>
                       </c:pt>
-                      <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>31.01</c:v>
                       </c:pt>
-                      <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>30.99</c:v>
                       </c:pt>
-                      <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>30.98</c:v>
                       </c:pt>
-                      <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>31.06</c:v>
                       </c:pt>
-                      <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>31.07</c:v>
                       </c:pt>
-                      <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>31.28</c:v>
                       </c:pt>
-                      <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>30.98</c:v>
                       </c:pt>
-                      <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>31</c:v>
                       </c:pt>
                     </c:numCache>
@@ -20545,7 +20518,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="359311744"/>
+        <c:axId val="196478448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20579,7 +20552,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359312136"/>
+        <c:crossAx val="196472464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -20587,7 +20560,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="359312136"/>
+        <c:axId val="196472464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20597,7 +20570,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="359311744"/>
+        <c:crossAx val="196478448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -20928,34 +20901,34 @@
                 <c:pt idx="2">
                   <c:v>1096.18</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1095.9000000000001</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>1093.69</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>1097.94</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>1097.6600000000001</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>1096.0999999999999</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>1097.76</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>1098.1300000000001</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>1107.5899999999999</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>1096.95</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>1096.03</c:v>
                 </c:pt>
               </c:numCache>
@@ -20994,8 +20967,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="359312920"/>
-        <c:axId val="359313312"/>
+        <c:axId val="196469200"/>
+        <c:axId val="196471376"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -21227,34 +21200,34 @@
                       <c:pt idx="2">
                         <c:v>816.77</c:v>
                       </c:pt>
-                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>815.36</c:v>
                       </c:pt>
-                      <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>815.4</c:v>
                       </c:pt>
-                      <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>816.88</c:v>
                       </c:pt>
-                      <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>817.12</c:v>
                       </c:pt>
-                      <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>817.16</c:v>
                       </c:pt>
-                      <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>819.04</c:v>
                       </c:pt>
-                      <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>819.48</c:v>
                       </c:pt>
-                      <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>821.15</c:v>
                       </c:pt>
-                      <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>817.92</c:v>
                       </c:pt>
-                      <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>818.37</c:v>
                       </c:pt>
                     </c:numCache>
@@ -21492,34 +21465,34 @@
                       <c:pt idx="2">
                         <c:v>620.38</c:v>
                       </c:pt>
-                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>618.64</c:v>
                       </c:pt>
-                      <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>617.87</c:v>
                       </c:pt>
-                      <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>620.35</c:v>
                       </c:pt>
-                      <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>619.9</c:v>
                       </c:pt>
-                      <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>619.79</c:v>
                       </c:pt>
-                      <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>621.29</c:v>
                       </c:pt>
-                      <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>621.5</c:v>
                       </c:pt>
-                      <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>625.62</c:v>
                       </c:pt>
-                      <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>619.64</c:v>
                       </c:pt>
-                      <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>620.16999999999996</c:v>
                       </c:pt>
                     </c:numCache>
@@ -21532,7 +21505,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="359312920"/>
+        <c:axId val="196469200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21566,7 +21539,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359313312"/>
+        <c:crossAx val="196471376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -21574,7 +21547,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="359313312"/>
+        <c:axId val="196471376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21584,7 +21557,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="359312920"/>
+        <c:crossAx val="196469200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -21915,34 +21888,34 @@
                 <c:pt idx="2">
                   <c:v>620.38</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>618.64</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>617.87</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>620.35</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>619.9</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>619.79</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>621.29</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>621.5</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>625.62</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>619.64</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>620.16999999999996</c:v>
                 </c:pt>
               </c:numCache>
@@ -21981,8 +21954,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="359314096"/>
-        <c:axId val="359759584"/>
+        <c:axId val="196477360"/>
+        <c:axId val="196474640"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -22214,34 +22187,34 @@
                       <c:pt idx="2">
                         <c:v>816.77</c:v>
                       </c:pt>
-                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>815.36</c:v>
                       </c:pt>
-                      <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>815.4</c:v>
                       </c:pt>
-                      <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>816.88</c:v>
                       </c:pt>
-                      <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>817.12</c:v>
                       </c:pt>
-                      <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>817.16</c:v>
                       </c:pt>
-                      <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>819.04</c:v>
                       </c:pt>
-                      <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>819.48</c:v>
                       </c:pt>
-                      <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>821.15</c:v>
                       </c:pt>
-                      <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>817.92</c:v>
                       </c:pt>
-                      <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>818.37</c:v>
                       </c:pt>
                     </c:numCache>
@@ -22479,34 +22452,34 @@
                       <c:pt idx="2">
                         <c:v>1096.18</c:v>
                       </c:pt>
-                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1095.9000000000001</c:v>
                       </c:pt>
-                      <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>1093.69</c:v>
                       </c:pt>
-                      <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>1097.94</c:v>
                       </c:pt>
-                      <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>1097.6600000000001</c:v>
                       </c:pt>
-                      <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>1096.0999999999999</c:v>
                       </c:pt>
-                      <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>1097.76</c:v>
                       </c:pt>
-                      <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>1098.1300000000001</c:v>
                       </c:pt>
-                      <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>1107.5899999999999</c:v>
                       </c:pt>
-                      <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>1096.95</c:v>
                       </c:pt>
-                      <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>1096.03</c:v>
                       </c:pt>
                     </c:numCache>
@@ -22519,7 +22492,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="359314096"/>
+        <c:axId val="196477360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22553,7 +22526,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359759584"/>
+        <c:crossAx val="196474640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -22561,7 +22534,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="359759584"/>
+        <c:axId val="196474640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22571,7 +22544,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="359314096"/>
+        <c:crossAx val="196477360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -22904,34 +22877,34 @@
                 <c:pt idx="2">
                   <c:v>51.45</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>51.44</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>51.51</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>51.55</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>51.57</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>51.69</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>51.77</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>51.78</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>51.96</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>51.77</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>51.84</c:v>
                 </c:pt>
               </c:numCache>
@@ -22970,11 +22943,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="356587056"/>
-        <c:axId val="234806784"/>
+        <c:axId val="289801200"/>
+        <c:axId val="289799568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="356587056"/>
+        <c:axId val="289801200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23008,7 +22981,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="234806784"/>
+        <c:crossAx val="289799568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -23016,7 +22989,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="234806784"/>
+        <c:axId val="289799568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23026,7 +22999,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="356587056"/>
+        <c:crossAx val="289801200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -23358,34 +23331,34 @@
                 <c:pt idx="2">
                   <c:v>816.77</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>815.36</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>815.4</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>816.88</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>817.12</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>817.16</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>819.04</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>819.48</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>821.15</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>817.92</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>818.37</c:v>
                 </c:pt>
               </c:numCache>
@@ -23424,8 +23397,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="359760368"/>
-        <c:axId val="359760760"/>
+        <c:axId val="196478992"/>
+        <c:axId val="196464848"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -23657,34 +23630,34 @@
                       <c:pt idx="2">
                         <c:v>620.38</c:v>
                       </c:pt>
-                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>618.64</c:v>
                       </c:pt>
-                      <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>617.87</c:v>
                       </c:pt>
-                      <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>620.35</c:v>
                       </c:pt>
-                      <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>619.9</c:v>
                       </c:pt>
-                      <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>619.79</c:v>
                       </c:pt>
-                      <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>621.29</c:v>
                       </c:pt>
-                      <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>621.5</c:v>
                       </c:pt>
-                      <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>625.62</c:v>
                       </c:pt>
-                      <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>619.64</c:v>
                       </c:pt>
-                      <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>620.16999999999996</c:v>
                       </c:pt>
                     </c:numCache>
@@ -23922,34 +23895,34 @@
                       <c:pt idx="2">
                         <c:v>1096.18</c:v>
                       </c:pt>
-                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1095.9000000000001</c:v>
                       </c:pt>
-                      <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>1093.69</c:v>
                       </c:pt>
-                      <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>1097.94</c:v>
                       </c:pt>
-                      <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>1097.6600000000001</c:v>
                       </c:pt>
-                      <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>1096.0999999999999</c:v>
                       </c:pt>
-                      <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>1097.76</c:v>
                       </c:pt>
-                      <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>1098.1300000000001</c:v>
                       </c:pt>
-                      <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>1107.5899999999999</c:v>
                       </c:pt>
-                      <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>1096.95</c:v>
                       </c:pt>
-                      <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>1096.03</c:v>
                       </c:pt>
                     </c:numCache>
@@ -23962,7 +23935,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="359760368"/>
+        <c:axId val="196478992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23996,7 +23969,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359760760"/>
+        <c:crossAx val="196464848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -24004,7 +23977,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="359760760"/>
+        <c:axId val="196464848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24014,7 +23987,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="359760368"/>
+        <c:crossAx val="196478992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -24422,11 +24395,11 @@
         </c:dropLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="359761152"/>
-        <c:axId val="359761936"/>
+        <c:axId val="196477904"/>
+        <c:axId val="196475184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="359761152"/>
+        <c:axId val="196477904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24460,7 +24433,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359761936"/>
+        <c:crossAx val="196475184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -24468,7 +24441,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="359761936"/>
+        <c:axId val="196475184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24478,7 +24451,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="359761152"/>
+        <c:crossAx val="196477904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -24781,34 +24754,34 @@
                 <c:pt idx="2">
                   <c:v>100.42</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>100.45</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>100.47</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>100.5</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>100.52</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>100.55</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>100.57</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>100.6</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>100.62</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>100.65</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>100.67</c:v>
                 </c:pt>
               </c:numCache>
@@ -24847,11 +24820,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="359762720"/>
-        <c:axId val="359763112"/>
+        <c:axId val="196467024"/>
+        <c:axId val="196471920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="359762720"/>
+        <c:axId val="196467024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24885,7 +24858,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359763112"/>
+        <c:crossAx val="196471920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -24893,7 +24866,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="359763112"/>
+        <c:axId val="196471920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24903,7 +24876,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="359762720"/>
+        <c:crossAx val="196467024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -25206,34 +25179,34 @@
                 <c:pt idx="2">
                   <c:v>10042.879999999999</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>10045.36</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>10047.84</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>10050.32</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>10052.799999999999</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>10055.290000000001</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>10057.77</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>10060.25</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>10062.74</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>10065.219999999999</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>10067.709999999999</c:v>
                 </c:pt>
               </c:numCache>
@@ -25272,11 +25245,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="359859984"/>
-        <c:axId val="359860376"/>
+        <c:axId val="196476816"/>
+        <c:axId val="196467568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="359859984"/>
+        <c:axId val="196476816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25310,7 +25283,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359860376"/>
+        <c:crossAx val="196467568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -25318,7 +25291,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="359860376"/>
+        <c:axId val="196467568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25328,7 +25301,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="359859984"/>
+        <c:crossAx val="196476816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -25633,34 +25606,34 @@
                 <c:pt idx="2">
                   <c:v>31.34</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>31.32</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>31.29</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>31.25</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>31.41</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>31.58</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>31.64</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>31.55</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>31.95</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>31.72</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>31.95</c:v>
                 </c:pt>
               </c:numCache>
@@ -25699,11 +25672,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="355865608"/>
-        <c:axId val="357548720"/>
+        <c:axId val="289795216"/>
+        <c:axId val="289799024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="355865608"/>
+        <c:axId val="289795216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25737,7 +25710,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="357548720"/>
+        <c:crossAx val="289799024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -25745,7 +25718,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="357548720"/>
+        <c:axId val="289799024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25755,7 +25728,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="355865608"/>
+        <c:crossAx val="289795216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -26089,34 +26062,34 @@
                 <c:pt idx="2">
                   <c:v>1567.44</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1566.45</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>1564.61</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>1562.77</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>1570.53</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>1579.18</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>1582.16</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>1577.88</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>1597.9</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>1586.27</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>1597.67</c:v>
                 </c:pt>
               </c:numCache>
@@ -26155,11 +26128,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="356801032"/>
-        <c:axId val="356586472"/>
+        <c:axId val="289800656"/>
+        <c:axId val="289795760"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="356801032"/>
+        <c:axId val="289800656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -26193,7 +26166,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="356586472"/>
+        <c:crossAx val="289795760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -26201,7 +26174,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="356586472"/>
+        <c:axId val="289795760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -26211,7 +26184,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="356801032"/>
+        <c:crossAx val="289800656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -26545,34 +26518,34 @@
                 <c:pt idx="2">
                   <c:v>1004.78</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1003.19</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>1001.05</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>998.93</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>1006.76</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>1015.21</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>1018.1</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>1013.41</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>1034.1300000000001</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>1021.72</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>1032.99</c:v>
                 </c:pt>
               </c:numCache>
@@ -26611,11 +26584,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="357141728"/>
-        <c:axId val="357142120"/>
+        <c:axId val="289804464"/>
+        <c:axId val="289805008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="357141728"/>
+        <c:axId val="289804464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -26649,7 +26622,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="357142120"/>
+        <c:crossAx val="289805008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -26657,7 +26630,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="357142120"/>
+        <c:axId val="289805008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -26667,7 +26640,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="357141728"/>
+        <c:crossAx val="289804464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -26759,6 +26732,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -26863,6 +26837,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -26999,34 +26974,34 @@
                 <c:pt idx="2">
                   <c:v>2572.5100000000002</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>2572.17</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>2575.6799999999998</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>2577.88</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>2578.7600000000002</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>2584.98</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>2588.5</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>2589.38</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>2598.1799999999998</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>2588.5100000000002</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                   <c:v>2592.4899999999998</c:v>
                 </c:pt>
               </c:numCache>
@@ -27065,8 +27040,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="357142904"/>
-        <c:axId val="357143296"/>
+        <c:axId val="289794672"/>
+        <c:axId val="289794128"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -27298,34 +27273,34 @@
                       <c:pt idx="2">
                         <c:v>1567.44</c:v>
                       </c:pt>
-                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1566.45</c:v>
                       </c:pt>
-                      <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>1564.61</c:v>
                       </c:pt>
-                      <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>1562.77</c:v>
                       </c:pt>
-                      <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>1570.53</c:v>
                       </c:pt>
-                      <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>1579.18</c:v>
                       </c:pt>
-                      <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>1582.16</c:v>
                       </c:pt>
-                      <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>1577.88</c:v>
                       </c:pt>
-                      <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>1597.9</c:v>
                       </c:pt>
-                      <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>1586.27</c:v>
                       </c:pt>
-                      <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>1597.67</c:v>
                       </c:pt>
                     </c:numCache>
@@ -27563,34 +27538,34 @@
                       <c:pt idx="2">
                         <c:v>1004.78</c:v>
                       </c:pt>
-                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00">
+                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1003.19</c:v>
                       </c:pt>
-                      <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="4" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>1001.05</c:v>
                       </c:pt>
-                      <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="5" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>998.93</c:v>
                       </c:pt>
-                      <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="6" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>1006.76</c:v>
                       </c:pt>
-                      <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="7" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>1015.21</c:v>
                       </c:pt>
-                      <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>1018.1</c:v>
                       </c:pt>
-                      <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="9" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>1013.41</c:v>
                       </c:pt>
-                      <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="10" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>1034.1300000000001</c:v>
                       </c:pt>
-                      <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="11" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>1021.72</c:v>
                       </c:pt>
-                      <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                      <c:pt idx="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00">
                         <c:v>1032.99</c:v>
                       </c:pt>
                     </c:numCache>
@@ -27603,7 +27578,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="357142904"/>
+        <c:axId val="289794672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -27637,7 +27612,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="357143296"/>
+        <c:crossAx val="289794128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -27645,7 +27620,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="357143296"/>
+        <c:axId val="289794128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -27655,7 +27630,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="357142904"/>
+        <c:crossAx val="289794672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -27669,6 +27644,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -28054,8 +28030,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="357141336"/>
-        <c:axId val="357144080"/>
+        <c:axId val="289806096"/>
+        <c:axId val="289808816"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -28592,7 +28568,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="357141336"/>
+        <c:axId val="289806096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -28626,7 +28602,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="357144080"/>
+        <c:crossAx val="289808816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -28634,7 +28610,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="357144080"/>
+        <c:axId val="289808816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -28644,7 +28620,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="357141336"/>
+        <c:crossAx val="289806096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -29044,8 +29020,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="357144864"/>
-        <c:axId val="357776728"/>
+        <c:axId val="289802288"/>
+        <c:axId val="175747568"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -29582,7 +29558,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="357144864"/>
+        <c:axId val="289802288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -29616,7 +29592,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="357776728"/>
+        <c:crossAx val="175747568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -29624,7 +29600,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="357776728"/>
+        <c:axId val="175747568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -29634,7 +29610,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="357144864"/>
+        <c:crossAx val="289802288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -53555,7 +53531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="O2" sqref="O2:AO3"/>
     </sheetView>
   </sheetViews>

</xml_diff>